<commit_message>
Adding Unit 2.1 materials
</commit_message>
<xml_diff>
--- a/01-Class-Activities/01-Excel/4/Activities/03-Ins_Variance-SD-Zscore/Solved/Variance-SD-Zscore.xlsx
+++ b/01-Class-Activities/01-Excel/4/Activities/03-Ins_Variance-SD-Zscore/Solved/Variance-SD-Zscore.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joekaplan/git/DataViz-Lesson-Plans/01-Lesson-Plans/01-Excel/3/Activities/08-Ins_Variance-SD-Zscore/Solved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98452\gwu-arl-data-pt-09-2020-u-c\01-Class-Activities\01-Excel\4\Activities\03-Ins_Variance-SD-Zscore\Solved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A970A051-7AAD-1248-A73C-A78AED6D112C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="45880" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="45880" windowHeight="28340" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Variance Example" sheetId="1" r:id="rId1"/>
@@ -18,11 +17,7 @@
     <sheet name="Normal Distribution 68%" sheetId="3" r:id="rId3"/>
     <sheet name="Z-Score" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Standard Deviation'!$B$2:$B$13</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Standard Deviation'!$B$2:$B$13</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -112,10 +107,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -213,22 +208,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="173" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -262,7 +257,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{D49F0EF7-EFF3-4B63-86D0-01C41125D719}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -322,6 +317,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -726,6 +722,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -757,6 +754,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -764,7 +762,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -843,6 +840,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1247,6 +1245,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1278,6 +1277,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1285,7 +1285,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2786,21 +2785,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="5.6640625" customWidth="1"/>
-    <col min="14" max="14" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="5.6328125" customWidth="1"/>
+    <col min="14" max="14" width="4.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2821,7 +2822,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2843,7 +2844,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2855,7 +2856,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2867,7 +2868,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2879,7 +2880,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2891,7 +2892,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2903,7 +2904,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2915,7 +2916,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2927,7 +2928,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2939,7 +2940,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2951,7 +2952,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2963,7 +2964,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
@@ -2975,7 +2976,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
@@ -2988,7 +2989,7 @@
         <v>7.0374015748031509</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
@@ -3008,21 +3009,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059EBE5-0310-C848-B2D5-24C533C74289}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="5.6640625" customWidth="1"/>
-    <col min="14" max="14" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="5.6328125" customWidth="1"/>
+    <col min="14" max="14" width="4.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3041,7 +3044,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3061,7 +3064,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3073,7 +3076,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3085,7 +3088,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3097,7 +3100,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3109,7 +3112,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3121,7 +3124,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3133,7 +3136,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3145,7 +3148,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3157,7 +3160,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3169,7 +3172,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3181,7 +3184,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
@@ -3193,7 +3196,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>7.0374015748031509</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
@@ -3219,7 +3222,7 @@
         <v>11.043287711575411</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>17</v>
       </c>
@@ -3232,7 +3235,7 @@
         <v>3.3231442507925251</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
@@ -3252,19 +3255,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC96B052-8719-5B49-B651-F0C0E6F0D800}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3275,7 +3278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>10.511811023622048</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>10.275590551181102</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3308,7 +3311,7 @@
         <v>11.614173228346457</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3319,7 +3322,7 @@
         <v>11.102362204724409</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3330,7 +3333,7 @@
         <v>8.2677165354330704</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>4.2913385826771657</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3352,7 +3355,7 @@
         <v>2.9921259842519685</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>2.204724409448819</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3374,7 +3377,7 @@
         <v>3.0314960629921264</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3385,7 +3388,7 @@
         <v>4.9212598425196852</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3396,7 +3399,7 @@
         <v>6.4960629921259843</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
@@ -3407,7 +3410,7 @@
         <v>8.7401574803149611</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
@@ -3422,7 +3425,7 @@
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
@@ -3437,14 +3440,14 @@
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
@@ -3459,7 +3462,7 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>21</v>
       </c>
@@ -3474,630 +3477,630 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="9"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="9"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="9"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="9"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="9"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="9"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="9"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="9"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="9"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="9"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="9"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="9"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="9"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="9"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="9"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="9"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="9"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="9"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="9"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="9"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="9"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="9"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="9"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="9"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="9"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="9"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="9"/>
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="9"/>
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="9"/>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="9"/>
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="9"/>
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
       <c r="D107" s="9"/>
       <c r="E107" s="9"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="9"/>
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
@@ -4110,21 +4113,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2F82B8-EBB9-F84F-B4C6-BC6A69F8B770}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4141,7 +4144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4160,7 +4163,7 @@
         <v>1.0455186975378206</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4179,7 +4182,7 @@
         <v>0.97443527334261415</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4198,7 +4201,7 @@
         <v>1.3772413437821149</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4217,7 +4220,7 @@
         <v>1.223227258025835</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4236,7 +4239,7 @@
         <v>0.37022616768336375</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4255,7 +4258,7 @@
         <v>-0.82634480626926932</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4274,7 +4277,7 @@
         <v>-1.217303639342902</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4293,7 +4296,7 @@
         <v>-1.4542483866602549</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4312,7 +4315,7 @@
         <v>-1.2054564019770342</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4331,7 +4334,7 @@
         <v>-0.63678900841538688</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>11</v>
       </c>
@@ -4350,7 +4353,7 @@
         <v>-0.16289951378068065</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
@@ -4369,7 +4372,7 @@
         <v>0.51239301607377585</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
@@ -4385,7 +4388,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
@@ -4401,7 +4404,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -4409,7 +4412,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -4417,7 +4420,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -4425,7 +4428,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -4433,7 +4436,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -4441,7 +4444,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -4449,7 +4452,7 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -4457,7 +4460,7 @@
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -4465,7 +4468,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -4473,7 +4476,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -4481,7 +4484,7 @@
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -4489,7 +4492,7 @@
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -4497,7 +4500,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -4505,7 +4508,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -4513,7 +4516,7 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -4521,7 +4524,7 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -4529,7 +4532,7 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -4537,7 +4540,7 @@
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -4545,7 +4548,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -4553,7 +4556,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -4561,7 +4564,7 @@
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -4569,7 +4572,7 @@
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -4577,7 +4580,7 @@
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -4585,7 +4588,7 @@
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="9"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -4593,7 +4596,7 @@
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="9"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -4601,7 +4604,7 @@
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="9"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -4609,7 +4612,7 @@
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="9"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -4617,7 +4620,7 @@
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="9"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -4625,7 +4628,7 @@
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="9"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -4633,7 +4636,7 @@
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="9"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -4641,7 +4644,7 @@
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="9"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -4649,7 +4652,7 @@
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="9"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -4657,7 +4660,7 @@
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="9"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -4665,7 +4668,7 @@
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="9"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -4673,7 +4676,7 @@
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="9"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -4681,7 +4684,7 @@
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="9"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -4689,7 +4692,7 @@
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -4697,7 +4700,7 @@
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="9"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
@@ -4705,7 +4708,7 @@
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="9"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -4713,7 +4716,7 @@
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -4721,7 +4724,7 @@
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -4729,7 +4732,7 @@
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="9"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -4737,7 +4740,7 @@
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -4745,7 +4748,7 @@
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -4753,7 +4756,7 @@
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -4761,7 +4764,7 @@
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -4769,7 +4772,7 @@
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -4777,7 +4780,7 @@
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -4785,7 +4788,7 @@
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -4793,7 +4796,7 @@
       <c r="E64" s="9"/>
       <c r="F64" s="9"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -4801,7 +4804,7 @@
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -4809,7 +4812,7 @@
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -4817,7 +4820,7 @@
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -4825,7 +4828,7 @@
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -4833,7 +4836,7 @@
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -4841,7 +4844,7 @@
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -4849,7 +4852,7 @@
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -4857,7 +4860,7 @@
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -4865,7 +4868,7 @@
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -4873,7 +4876,7 @@
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -4881,7 +4884,7 @@
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -4889,7 +4892,7 @@
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -4897,7 +4900,7 @@
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -4905,7 +4908,7 @@
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -4913,7 +4916,7 @@
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -4921,7 +4924,7 @@
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -4929,7 +4932,7 @@
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -4937,7 +4940,7 @@
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -4945,7 +4948,7 @@
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -4953,7 +4956,7 @@
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -4961,7 +4964,7 @@
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
@@ -4969,7 +4972,7 @@
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -4977,7 +4980,7 @@
       <c r="E87" s="9"/>
       <c r="F87" s="9"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -4985,7 +4988,7 @@
       <c r="E88" s="9"/>
       <c r="F88" s="9"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -4993,7 +4996,7 @@
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -5001,7 +5004,7 @@
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="9"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -5009,7 +5012,7 @@
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="9"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -5017,7 +5020,7 @@
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="9"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -5025,7 +5028,7 @@
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="9"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -5033,7 +5036,7 @@
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="9"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -5041,7 +5044,7 @@
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -5049,7 +5052,7 @@
       <c r="E96" s="9"/>
       <c r="F96" s="9"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="9"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -5057,7 +5060,7 @@
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="9"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -5065,7 +5068,7 @@
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="9"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
@@ -5073,7 +5076,7 @@
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="9"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -5081,7 +5084,7 @@
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="9"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -5089,7 +5092,7 @@
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -5097,7 +5100,7 @@
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="9"/>
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
@@ -5105,7 +5108,7 @@
       <c r="E103" s="9"/>
       <c r="F103" s="9"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="9"/>
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
@@ -5113,7 +5116,7 @@
       <c r="E104" s="9"/>
       <c r="F104" s="9"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="9"/>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
@@ -5121,7 +5124,7 @@
       <c r="E105" s="9"/>
       <c r="F105" s="9"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="9"/>
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
@@ -5129,7 +5132,7 @@
       <c r="E106" s="9"/>
       <c r="F106" s="9"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="9"/>
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
@@ -5137,7 +5140,7 @@
       <c r="E107" s="9"/>
       <c r="F107" s="9"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="9"/>
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>

</xml_diff>